<commit_message>
Funcionalidade recomendacao de investimento
</commit_message>
<xml_diff>
--- a/dados_magic_formula.xlsx
+++ b/dados_magic_formula.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Preco</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Recomendação Investimento</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,6 +505,9 @@
       <c r="G2" t="n">
         <v>34.13999938964844</v>
       </c>
+      <c r="H2" t="n">
+        <v>1024.199981689453</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -531,6 +539,9 @@
       <c r="G3" t="n">
         <v>6.269999980926514</v>
       </c>
+      <c r="H3" t="n">
+        <v>188.0999994277954</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -562,6 +573,9 @@
       <c r="G4" t="n">
         <v>12.27999973297119</v>
       </c>
+      <c r="H4" t="n">
+        <v>356.1199922561646</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -593,6 +607,9 @@
       <c r="G5" t="n">
         <v>5.550000190734863</v>
       </c>
+      <c r="H5" t="n">
+        <v>160.950005531311</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -624,6 +641,9 @@
       <c r="G6" t="n">
         <v>39.38999938964844</v>
       </c>
+      <c r="H6" t="n">
+        <v>1142.309982299805</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -655,6 +675,9 @@
       <c r="G7" t="n">
         <v>36.88999938964844</v>
       </c>
+      <c r="H7" t="n">
+        <v>1069.809982299805</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -686,6 +709,9 @@
       <c r="G8" t="n">
         <v>57.40000152587891</v>
       </c>
+      <c r="H8" t="n">
+        <v>1664.600044250488</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -717,6 +743,9 @@
       <c r="G9" t="n">
         <v>22.17000007629395</v>
       </c>
+      <c r="H9" t="n">
+        <v>642.9300022125244</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -748,6 +777,9 @@
       <c r="G10" t="n">
         <v>3.890000104904175</v>
       </c>
+      <c r="H10" t="n">
+        <v>116.7000031471252</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -779,6 +811,9 @@
       <c r="G11" t="n">
         <v>31.45000076293945</v>
       </c>
+      <c r="H11" t="n">
+        <v>912.0500221252441</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -810,6 +845,9 @@
       <c r="G12" t="n">
         <v>47.04999923706055</v>
       </c>
+      <c r="H12" t="n">
+        <v>1364.449977874756</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -841,6 +879,9 @@
       <c r="G13" t="n">
         <v>11.51000022888184</v>
       </c>
+      <c r="H13" t="n">
+        <v>333.7900066375732</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -872,6 +913,9 @@
       <c r="G14" t="n">
         <v>9.729999542236328</v>
       </c>
+      <c r="H14" t="n">
+        <v>282.1699867248535</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -903,6 +947,9 @@
       <c r="G15" t="n">
         <v>17.75</v>
       </c>
+      <c r="H15" t="n">
+        <v>514.75</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -934,6 +981,9 @@
       <c r="G16" t="n">
         <v>1.980000019073486</v>
       </c>
+      <c r="H16" t="n">
+        <v>57.4200005531311</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -965,6 +1015,9 @@
       <c r="G17" t="n">
         <v>18.79999923706055</v>
       </c>
+      <c r="H17" t="n">
+        <v>545.1999778747559</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -996,6 +1049,9 @@
       <c r="G18" t="n">
         <v>26.19000053405762</v>
       </c>
+      <c r="H18" t="n">
+        <v>759.5100154876709</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1027,6 +1083,9 @@
       <c r="G19" t="n">
         <v>3.859999895095825</v>
       </c>
+      <c r="H19" t="n">
+        <v>111.9399969577789</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1058,6 +1117,9 @@
       <c r="G20" t="n">
         <v>23.64999961853027</v>
       </c>
+      <c r="H20" t="n">
+        <v>685.8499889373779</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1089,6 +1151,9 @@
       <c r="G21" t="n">
         <v>25.45000076293945</v>
       </c>
+      <c r="H21" t="n">
+        <v>738.0500221252441</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1120,6 +1185,9 @@
       <c r="G22" t="n">
         <v>7.699999809265137</v>
       </c>
+      <c r="H22" t="n">
+        <v>223.299994468689</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1151,6 +1219,9 @@
       <c r="G23" t="n">
         <v>11.35000038146973</v>
       </c>
+      <c r="H23" t="n">
+        <v>329.1500110626221</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1182,6 +1253,9 @@
       <c r="G24" t="n">
         <v>24</v>
       </c>
+      <c r="H24" t="n">
+        <v>696</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1213,6 +1287,9 @@
       <c r="G25" t="n">
         <v>1.779999971389771</v>
       </c>
+      <c r="H25" t="n">
+        <v>51.61999917030334</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1244,6 +1321,9 @@
       <c r="G26" t="n">
         <v>11.27999973297119</v>
       </c>
+      <c r="H26" t="n">
+        <v>327.1199922561646</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1275,6 +1355,9 @@
       <c r="G27" t="n">
         <v>12.10000038146973</v>
       </c>
+      <c r="H27" t="n">
+        <v>350.9000110626221</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1306,6 +1389,9 @@
       <c r="G28" t="n">
         <v>4</v>
       </c>
+      <c r="H28" t="n">
+        <v>116</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1337,6 +1423,9 @@
       <c r="G29" t="n">
         <v>6.829999923706055</v>
       </c>
+      <c r="H29" t="n">
+        <v>198.0699977874756</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1368,6 +1457,9 @@
       <c r="G30" t="n">
         <v>10.55000019073486</v>
       </c>
+      <c r="H30" t="n">
+        <v>305.950005531311</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1398,6 +1490,9 @@
       </c>
       <c r="G31" t="n">
         <v>7.949999809265137</v>
+      </c>
+      <c r="H31" t="n">
+        <v>230.549994468689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>